<commit_message>
Update #A-1 -Added 1 testcase related to add SupplierDetailsTestCases
</commit_message>
<xml_diff>
--- a/InputData/Supplier_details.xlsx
+++ b/InputData/Supplier_details.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ManishaDrive\Prompt-Solutions-v1\InputData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="14690" windowHeight="6060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14685" windowHeight="6060"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:O19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t>Email</t>
   </si>
@@ -194,13 +198,31 @@
   </si>
   <si>
     <t xml:space="preserve">Supplier Source </t>
+  </si>
+  <si>
+    <t>sukanya@vtestcorp.com</t>
+  </si>
+  <si>
+    <t>sukanya@123</t>
+  </si>
+  <si>
+    <t>Quick 2019/11/27 18:27:05</t>
+  </si>
+  <si>
+    <t>www.quick.com</t>
+  </si>
+  <si>
+    <t>Software development</t>
+  </si>
+  <si>
+    <t>Dream City</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +278,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -302,7 +332,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -334,9 +364,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -368,6 +399,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -543,30 +575,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.140625" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.36328125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.453125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7265625" style="1" collapsed="1"/>
-    <col min="7" max="8" width="8.7265625" style="1"/>
-    <col min="9" max="15" width="8.7265625" style="1" collapsed="1"/>
-    <col min="16" max="16" width="10.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="35" width="8.7265625" style="1" collapsed="1"/>
-    <col min="36" max="38" width="8.7265625" style="1"/>
-    <col min="39" max="16384" width="8.7265625" style="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" collapsed="1"/>
+    <col min="7" max="8" width="8.7109375" style="1"/>
+    <col min="9" max="15" width="8.7109375" style="1" collapsed="1"/>
+    <col min="16" max="16" width="10.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="35" width="8.7109375" style="1" collapsed="1"/>
+    <col min="36" max="38" width="8.7109375" style="1"/>
+    <col min="39" max="16384" width="8.7109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="43.5">
+    <row r="1" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +705,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="29">
+    <row r="2" spans="1:35" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -774,6 +806,113 @@
         <v>48</v>
       </c>
       <c r="AH2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1">
+        <v>411011</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>7789066033</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="1">
+        <v>1234567</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1234567</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W3" s="1">
+        <v>1234567</v>
+      </c>
+      <c r="X3" s="1">
+        <v>1234567</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>100</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>199</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI3" s="1">
         <v>100</v>
       </c>
     </row>
@@ -783,32 +922,35 @@
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="Q2" r:id="rId3"/>
     <hyperlink ref="H2" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId5"/>
+    <hyperlink ref="R3" r:id="rId6"/>
+    <hyperlink ref="A3" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>